<commit_message>
feat: update Sprint 3 charts
</commit_message>
<xml_diff>
--- a/Docs/Iteración 3/MS Project/Seguimiento de Costes acumulado del Sprint 3.xlsx
+++ b/Docs/Iteración 3/MS Project/Seguimiento de Costes acumulado del Sprint 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\Universidad\4º AÑO\PGPI-G1.15\Docs\Iteración 3\MS Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E392951-9138-4700-9A4C-391D41C552C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{707275E7-0597-4126-83C6-BD19029F359F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1FBA0FEE-2E2B-44B7-A2EB-9404927FAE77}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05B1768D-A3C4-4EBF-A134-7FE507D84E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="2" r:id="rId1"/>
@@ -36,9 +36,9 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{5836961B-343F-43C7-A2C2-D78370D90745}" sourceFile="D:\Documents and Settings\PKMACCT\My Documents\Assignment Usage.cub" keepAlive="1" name="Assignment Usage" type="5" refreshedVersion="8">
+  <connection id="1" xr16:uid="{F8AAE1A6-DD8A-4105-B51B-1718B54299A6}" sourceFile="D:\Documents and Settings\PKMACCT\My Documents\Assignment Usage.cub" keepAlive="1" name="Assignment Usage" type="5" refreshedVersion="8">
     <dbPr connection="Provider=MSOLAP.2;Persist Security Info=True;Data Source=D:\Documents and Settings\PKMACCT\My Documents\Assignment Usage.cub;Client Cache Size=25;Auto Synch Period=10000" command="ProjectReport" commandType="1"/>
-    <olapPr local="1" localConnection="Provider=MSOLAP.8;Persist Security Info=True;Data Source=C:\Users\angel\AppData\Local\Temp\VisualReportsTemporaryData\{78b79d6a-3baf-ef11-905f-c38c60dbbcf3}\AssignmentTP.cub;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" rowDrillCount="1000" serverFill="0" serverNumberFormat="0" serverFont="0" serverFontColor="0"/>
+    <olapPr local="1" localConnection="Provider=MSOLAP.8;Persist Security Info=True;Data Source=C:\Users\angel\AppData\Local\Temp\VisualReportsTemporaryData\{4070da52-97b1-ef11-9061-9b9808f6d72a}\AssignmentTP.cub;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" rowDrillCount="1000" serverFill="0" serverNumberFormat="0" serverFont="0" serverFontColor="0"/>
   </connection>
 </connections>
 </file>
@@ -101,6 +101,9 @@
     <t>Total 2024</t>
   </si>
   <si>
+    <t>Costo de línea base</t>
+  </si>
+  <si>
     <t>Semana</t>
   </si>
   <si>
@@ -141,9 +144,6 @@
   </si>
   <si>
     <t>Total T3</t>
-  </si>
-  <si>
-    <t>Costo de línea base</t>
   </si>
   <si>
     <t>Costo acumulado</t>
@@ -406,15 +406,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Informe de costo presupuestado</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> acumulado </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>del Sprint 3</a:t>
+              <a:t>Informe de costo presupuestado acumulado del Sprint 3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -607,7 +599,7 @@
                   <c:v>507.56774193548392</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>592.56774193548392</c:v>
+                  <c:v>666.56774193548392</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>307.72514112903224</c:v>
@@ -623,7 +615,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9872-4D2F-9001-083E92F9BB46}"/>
+              <c16:uniqueId val="{00000000-2847-45D5-AF19-42B72B3F4BC9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -742,7 +734,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9872-4D2F-9001-083E92F9BB46}"/>
+              <c16:uniqueId val="{00000005-2847-45D5-AF19-42B72B3F4BC9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -845,23 +837,23 @@
                   <c:v>2538.9377419354837</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3179.5054838709675</c:v>
+                  <c:v>3205.5054838709675</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3518.443116883117</c:v>
+                  <c:v>3544.443116883117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5159.5700000000006</c:v>
+                  <c:v>5185.5700000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5570.0800000000008</c:v>
+                  <c:v>5596.0800000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-9872-4D2F-9001-083E92F9BB46}"/>
+              <c16:uniqueId val="{00000006-2847-45D5-AF19-42B72B3F4BC9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -874,11 +866,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="724377200"/>
+        <c:axId val="1863709983"/>
         <c:axId val="1"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="724377200"/>
+        <c:axId val="1863709983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,7 +939,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="724377200"/>
+        <c:crossAx val="1863709983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -975,7 +967,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{51A09193-4F36-4323-B83A-4441FAA399E5}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{FA7C66B8-2D32-46B5-980C-922ED1A360AE}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
@@ -997,7 +989,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39EF306B-4FF2-EF98-0010-8BE3FBA6BA3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97A536B1-200C-F40F-F381-FAE2F4A09142}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1021,7 +1013,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Angel Garcia" refreshedDate="45626.74533946759" createdVersion="8" refreshedVersion="8" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{F94F01D1-783D-422B-A5B5-1878F748C655}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Angel Garcia" refreshedDate="45629.74710104167" createdVersion="8" refreshedVersion="8" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{BFCD2C39-8230-4DF4-A2F8-7BCAA3F8DACF}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="49">
     <cacheField name="[Measures].[Costo real]" caption="Costo real" numFmtId="0" hierarchy="68"/>
@@ -1325,7 +1317,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0C35061B-81D4-470E-8C04-6F67D13475CB}" name="PivotTable1" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Datos" grandTotalCaption="Total general" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C877C5E7-D3D8-43E5-9C39-EC6F9D02D1BF}" name="PivotTable1" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Datos" grandTotalCaption="Total general" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" chartFormat="1" fieldListSortAscending="1">
   <location ref="A3:F19" firstHeaderRow="1" firstDataRow="2" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField name="Costo real" dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -1937,7 +1929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EC4604-5F7A-4EFF-9DCA-444100F56460}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096EC807-E476-48BE-952C-BC92E974082F}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1982,13 +1974,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>26</v>
@@ -2002,7 +1994,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="7">
         <v>3.8345038167938932</v>
@@ -2017,7 +2009,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="7">
@@ -2036,7 +2028,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="7">
         <v>6.3908396946564894</v>
@@ -2052,7 +2044,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="12">
         <v>6.3908396946564885</v>
@@ -2068,7 +2060,7 @@
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="12">
         <v>778.38838469512768</v>
@@ -2084,7 +2076,7 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="12">
         <v>386.6864197530864</v>
@@ -2100,7 +2092,7 @@
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="12">
         <v>849.6790123456791</v>
@@ -2116,7 +2108,7 @@
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="12">
         <v>507.56774193548392</v>
@@ -2132,23 +2124,23 @@
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" s="12">
-        <v>592.56774193548392</v>
+        <v>666.56774193548392</v>
       </c>
       <c r="E13" s="13">
         <v>1951.5677419354838</v>
       </c>
       <c r="F13" s="14">
-        <v>3179.5054838709675</v>
+        <v>3205.5054838709675</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="12">
         <v>307.72514112903224</v>
@@ -2157,14 +2149,14 @@
         <v>1415.567741935484</v>
       </c>
       <c r="F14" s="14">
-        <v>3518.443116883117</v>
+        <v>3544.443116883117</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="12">
         <v>367.36259111111116</v>
@@ -2173,14 +2165,14 @@
         <v>3147.4967741935484</v>
       </c>
       <c r="F15" s="14">
-        <v>5159.5700000000006</v>
+        <v>5185.5700000000006</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="12">
         <v>0</v>
@@ -2189,23 +2181,23 @@
         <v>410.51</v>
       </c>
       <c r="F16" s="14">
-        <v>5570.0800000000008</v>
+        <v>5596.0800000000008</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="7">
-        <v>3802.7587122943178</v>
+        <v>3876.7587122943178</v>
       </c>
       <c r="E17" s="8">
         <v>10142.274545454544</v>
       </c>
       <c r="F17" s="9">
-        <v>5570.0800000000008</v>
+        <v>5596.0800000000008</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -2215,13 +2207,13 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="7">
-        <v>3806.5932161111118</v>
+        <v>3880.5932161111118</v>
       </c>
       <c r="E18" s="8">
         <v>10146.079999999998</v>
       </c>
       <c r="F18" s="9">
-        <v>5570.0800000000008</v>
+        <v>5596.0800000000008</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -2231,13 +2223,13 @@
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17">
-        <v>3806.5932161111118</v>
+        <v>3880.5932161111118</v>
       </c>
       <c r="E19" s="18">
         <v>10146.079999999998</v>
       </c>
       <c r="F19" s="19">
-        <v>5570.0800000000008</v>
+        <v>5596.0800000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>